<commit_message>
feat: better spreadsheet management
</commit_message>
<xml_diff>
--- a/test/resources/datasets/dates.xlsx
+++ b/test/resources/datasets/dates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">colstr</t>
   </si>
@@ -33,6 +33,9 @@
   <si>
     <t xml:space="preserve">val2</t>
   </si>
+  <si>
+    <t xml:space="preserve">val3</t>
+  </si>
 </sst>
 </file>
 
@@ -40,13 +43,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,8 +110,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -132,36 +140,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>44169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>44170</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>